<commit_message>
added future power plant fuel prices expectations
</commit_message>
<xml_diff>
--- a/data/TradeRES_D2_1_Scenario_data_Corrected (1).xlsx
+++ b/data/TradeRES_D2_1_Scenario_data_Corrected (1).xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD179B2-B72D-4548-BA6A-0EC33B5F6496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5156885B-D11C-471F-AE37-C26A8A80AD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="460" yWindow="430" windowWidth="14400" windowHeight="7370" tabRatio="903" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="903" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
     <sheet name="Index" sheetId="4" r:id="rId2"/>
     <sheet name="Scenarios" sheetId="2" r:id="rId3"/>
     <sheet name="Emission_prices" sheetId="6" r:id="rId4"/>
-    <sheet name="Commodity_prices" sheetId="7" r:id="rId5"/>
+    <sheet name="Commodity_prices (2)" sheetId="15" r:id="rId5"/>
     <sheet name="New_technology_data" sheetId="8" r:id="rId6"/>
     <sheet name="New_transmission_data" sheetId="9" r:id="rId7"/>
     <sheet name="Biomass_potential" sheetId="10" r:id="rId8"/>
@@ -26,6 +26,9 @@
     <sheet name="Transmission_capacities" sheetId="13" r:id="rId11"/>
     <sheet name="Generation_capacities" sheetId="14" r:id="rId12"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">New_technology_data!$A$1:$BI$138</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -79,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3360" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3416" uniqueCount="620">
   <si>
     <t>Data sheets for the database of TradeRES scenarios</t>
   </si>
@@ -2422,6 +2425,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2431,11 +2439,6 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -5368,26 +5371,26 @@
       <c r="E1" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="73" t="s">
         <v>516</v>
       </c>
-      <c r="G1" s="70"/>
-      <c r="H1" s="68" t="s">
+      <c r="G1" s="73"/>
+      <c r="H1" s="71" t="s">
         <v>517</v>
       </c>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68" t="s">
+      <c r="I1" s="71"/>
+      <c r="J1" s="71" t="s">
         <v>518</v>
       </c>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68" t="s">
+      <c r="K1" s="71"/>
+      <c r="L1" s="71" t="s">
         <v>519</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68" t="s">
+      <c r="M1" s="71"/>
+      <c r="N1" s="71" t="s">
         <v>520</v>
       </c>
-      <c r="O1" s="68"/>
+      <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -10836,14 +10839,14 @@
       </c>
     </row>
     <row r="120" spans="1:15" ht="136.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="69" t="s">
+      <c r="A120" s="72" t="s">
         <v>560</v>
       </c>
-      <c r="B120" s="69"/>
-      <c r="C120" s="69"/>
-      <c r="D120" s="69"/>
-      <c r="E120" s="69"/>
-      <c r="F120" s="69"/>
+      <c r="B120" s="72"/>
+      <c r="C120" s="72"/>
+      <c r="D120" s="72"/>
+      <c r="E120" s="72"/>
+      <c r="F120" s="72"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G121" s="1" t="s">
@@ -22077,14 +22080,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294E0319-5F46-4D50-9263-53C4B82A0F5E}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -22146,7 +22152,7 @@
         <v>84</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I10" si="0">ROUND(E2*3.6,2)</f>
+        <f>ROUND(E2*3.6,2)</f>
         <v>1.69</v>
       </c>
       <c r="K2" t="s">
@@ -22170,7 +22176,7 @@
         <v>84</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I3:I11" si="0">ROUND(E3*3.6,2)</f>
         <v>3.96</v>
       </c>
       <c r="K3" t="s">
@@ -22501,6 +22507,427 @@
       <c r="K15" t="s">
         <v>103</v>
       </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="36">
+        <v>2020</v>
+      </c>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36">
+        <v>0.47</v>
+      </c>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36">
+        <f>ROUND(E17*3.6,2)</f>
+        <v>1.69</v>
+      </c>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36">
+        <f t="shared" ref="I18:I29" si="1">ROUND(E18*3.6,2)</f>
+        <v>3.96</v>
+      </c>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36">
+        <f t="shared" si="1"/>
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36">
+        <v>3</v>
+      </c>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36">
+        <f t="shared" si="1"/>
+        <v>10.8</v>
+      </c>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36">
+        <v>5.6</v>
+      </c>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36">
+        <f t="shared" si="1"/>
+        <v>20.16</v>
+      </c>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36">
+        <v>12.9</v>
+      </c>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36">
+        <f t="shared" si="1"/>
+        <v>46.44</v>
+      </c>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36">
+        <v>10.6</v>
+      </c>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36">
+        <f t="shared" si="1"/>
+        <v>38.159999999999997</v>
+      </c>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36">
+        <f>1.1*E21</f>
+        <v>6.16</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36">
+        <f t="shared" si="1"/>
+        <v>22.18</v>
+      </c>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36">
+        <f>1.5*E21</f>
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36">
+        <f t="shared" si="1"/>
+        <v>30.24</v>
+      </c>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="36">
+        <f>ROUND(H26/3.6,2)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36">
+        <f>ROUND(J26/3.6,2)</f>
+        <v>4.17</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="36">
+        <v>0</v>
+      </c>
+      <c r="I26" s="36">
+        <f>AVERAGE(H26,J26)</f>
+        <v>7.5</v>
+      </c>
+      <c r="J26" s="36">
+        <v>15</v>
+      </c>
+      <c r="K26" s="36"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="36">
+        <f>ROUND(H27/3.6,2)</f>
+        <v>4.17</v>
+      </c>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36">
+        <f>ROUND(J27/3.6,2)</f>
+        <v>8.33</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="36">
+        <v>15</v>
+      </c>
+      <c r="I27" s="36">
+        <f t="shared" ref="I27:I30" si="2">AVERAGE(H27,J27)</f>
+        <v>22.5</v>
+      </c>
+      <c r="J27" s="36">
+        <v>30</v>
+      </c>
+      <c r="K27" s="36"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="36">
+        <f>ROUND(H28/3.6,2)</f>
+        <v>8.33</v>
+      </c>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36">
+        <f>ROUND(J28/3.6,2)</f>
+        <v>12.5</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H28" s="36">
+        <v>30</v>
+      </c>
+      <c r="I28" s="36">
+        <f t="shared" si="2"/>
+        <v>37.5</v>
+      </c>
+      <c r="J28" s="36">
+        <v>45</v>
+      </c>
+      <c r="K28" s="36"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="36">
+        <f>ROUND(H29/3.6,2)</f>
+        <v>10</v>
+      </c>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36">
+        <f>ROUND(J29/3.6,2)</f>
+        <v>28.33</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29" s="36">
+        <v>36</v>
+      </c>
+      <c r="I29" s="36">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="J29" s="36">
+        <v>102</v>
+      </c>
+      <c r="K29" s="36"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="36">
+        <f>ROUND(H30/3.6,2)</f>
+        <v>11.11</v>
+      </c>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36">
+        <f>ROUND(J30/3.6,2)</f>
+        <v>34.72</v>
+      </c>
+      <c r="G30" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H30" s="36">
+        <v>40</v>
+      </c>
+      <c r="I30" s="36">
+        <f t="shared" si="2"/>
+        <v>82.5</v>
+      </c>
+      <c r="J30" s="36">
+        <v>125</v>
+      </c>
+      <c r="K30" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22509,19 +22936,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:BI138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G30" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:T2"/>
+      <selection pane="bottomRight" activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="3.75" style="2" customWidth="1"/>
-    <col min="3" max="6" width="3.75" customWidth="1"/>
+    <col min="1" max="2" width="13.58203125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="13.58203125" customWidth="1"/>
     <col min="7" max="7" width="6.58203125" customWidth="1"/>
     <col min="8" max="8" width="4.75" customWidth="1"/>
     <col min="9" max="9" width="6.58203125" customWidth="1"/>
@@ -22735,7 +23163,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:61" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:61" s="30" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G2" s="30" t="s">
         <v>151</v>
       </c>
@@ -22854,7 +23282,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>164</v>
       </c>
@@ -22997,7 +23425,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>164</v>
       </c>
@@ -23140,7 +23568,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>164</v>
       </c>
@@ -23283,7 +23711,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>176</v>
       </c>
@@ -23426,7 +23854,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>176</v>
       </c>
@@ -23569,7 +23997,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>176</v>
       </c>
@@ -23712,7 +24140,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>180</v>
       </c>
@@ -23850,7 +24278,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>180</v>
       </c>
@@ -23988,7 +24416,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>186</v>
       </c>
@@ -24126,7 +24554,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>186</v>
       </c>
@@ -24264,7 +24692,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>191</v>
       </c>
@@ -24404,7 +24832,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>191</v>
       </c>
@@ -24544,7 +24972,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>191</v>
       </c>
@@ -24684,7 +25112,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>198</v>
       </c>
@@ -24752,7 +25180,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>198</v>
       </c>
@@ -24820,7 +25248,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>198</v>
       </c>
@@ -24888,7 +25316,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>206</v>
       </c>
@@ -24956,7 +25384,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>206</v>
       </c>
@@ -25024,7 +25452,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>206</v>
       </c>
@@ -25092,7 +25520,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>210</v>
       </c>
@@ -25161,7 +25589,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>214</v>
       </c>
@@ -25230,7 +25658,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>216</v>
       </c>
@@ -25299,7 +25727,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>218</v>
       </c>
@@ -25367,7 +25795,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>210</v>
       </c>
@@ -25436,7 +25864,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>214</v>
       </c>
@@ -25505,7 +25933,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>216</v>
       </c>
@@ -25574,7 +26002,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>218</v>
       </c>
@@ -25642,7 +26070,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>210</v>
       </c>
@@ -25711,7 +26139,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>214</v>
       </c>
@@ -25780,7 +26208,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>216</v>
       </c>
@@ -25849,7 +26277,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>218</v>
       </c>
@@ -25920,7 +26348,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>221</v>
       </c>
@@ -25993,7 +26421,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>221</v>
       </c>
@@ -26065,7 +26493,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="36" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>224</v>
       </c>
@@ -26167,7 +26595,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>224</v>
       </c>
@@ -26269,7 +26697,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>227</v>
       </c>
@@ -26367,101 +26795,101 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="1:61" s="72" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="71" t="s">
+    <row r="39" spans="1:61" s="69" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="68" t="s">
         <v>227</v>
       </c>
-      <c r="B39" s="71" t="s">
+      <c r="B39" s="68" t="s">
         <v>165</v>
       </c>
-      <c r="C39" s="72" t="s">
+      <c r="C39" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="D39" s="72" t="s">
+      <c r="D39" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="E39" s="72">
+      <c r="E39" s="69">
         <v>2050</v>
       </c>
-      <c r="G39" s="72">
+      <c r="G39" s="69">
         <f>AVERAGE(100,500)</f>
         <v>300</v>
       </c>
-      <c r="H39" s="72" t="s">
+      <c r="H39" s="69" t="s">
         <v>228</v>
       </c>
-      <c r="I39" s="72">
+      <c r="I39" s="69">
         <v>800</v>
       </c>
-      <c r="J39" s="72" t="s">
+      <c r="J39" s="69" t="s">
         <v>229</v>
       </c>
-      <c r="K39" s="72">
+      <c r="K39" s="69">
         <v>26000</v>
       </c>
-      <c r="L39" s="72" t="s">
+      <c r="L39" s="69" t="s">
         <v>229</v>
       </c>
-      <c r="M39" s="72">
+      <c r="M39" s="69">
         <v>4</v>
       </c>
-      <c r="N39" s="72" t="s">
+      <c r="N39" s="69" t="s">
         <v>229</v>
       </c>
-      <c r="O39" s="72">
+      <c r="O39" s="69">
         <v>25</v>
       </c>
-      <c r="P39" s="72" t="s">
+      <c r="P39" s="69" t="s">
         <v>228</v>
       </c>
-      <c r="Q39" s="72">
+      <c r="Q39" s="69">
         <v>20</v>
       </c>
-      <c r="R39" s="72">
+      <c r="R39" s="69">
         <v>7</v>
       </c>
-      <c r="S39" s="73">
+      <c r="S39" s="70">
         <f t="shared" si="1"/>
         <v>9.4393000000000005E-2</v>
       </c>
-      <c r="T39" s="73">
+      <c r="T39" s="70">
         <f t="shared" si="0"/>
         <v>75514.400000000009</v>
       </c>
-      <c r="U39" s="72" t="s">
+      <c r="U39" s="69" t="s">
         <v>170</v>
       </c>
-      <c r="V39" s="72">
+      <c r="V39" s="69">
         <v>14</v>
       </c>
-      <c r="W39" s="72" t="s">
+      <c r="W39" s="69" t="s">
         <v>228</v>
       </c>
-      <c r="AF39" s="72">
+      <c r="AF39" s="69">
         <v>1</v>
       </c>
-      <c r="AG39" s="72">
+      <c r="AG39" s="69">
         <v>2</v>
       </c>
-      <c r="AK39" s="72">
+      <c r="AK39" s="69">
         <v>40</v>
       </c>
-      <c r="AL39" s="72" t="s">
+      <c r="AL39" s="69" t="s">
         <v>230</v>
       </c>
-      <c r="AM39" s="72">
+      <c r="AM39" s="69">
         <v>63</v>
       </c>
-      <c r="AP39" s="72" t="s">
+      <c r="AP39" s="69" t="s">
         <v>228</v>
       </c>
-      <c r="BA39" s="72" t="s">
+      <c r="BA39" s="69" t="s">
         <v>173</v>
       </c>
-      <c r="BB39" s="72">
+      <c r="BB39" s="69">
         <v>15</v>
       </c>
-      <c r="BF39" s="72" t="s">
+      <c r="BF39" s="69" t="s">
         <v>228</v>
       </c>
     </row>
@@ -26554,7 +26982,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:61" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:61" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="34" t="s">
         <v>232</v>
       </c>
@@ -26576,7 +27004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:61" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:61" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="34" t="s">
         <v>232</v>
       </c>
@@ -26598,7 +27026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:61" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:61" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="34" t="s">
         <v>232</v>
       </c>
@@ -26617,7 +27045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>236</v>
       </c>
@@ -26670,7 +27098,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>236</v>
       </c>
@@ -26723,7 +27151,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="46" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>241</v>
       </c>
@@ -26776,7 +27204,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="47" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>241</v>
       </c>
@@ -26829,7 +27257,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="48" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>244</v>
       </c>
@@ -26894,7 +27322,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:58" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>244</v>
       </c>
@@ -26959,7 +27387,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:58" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>247</v>
       </c>
@@ -27003,7 +27431,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:58" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>247</v>
       </c>
@@ -27047,7 +27475,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>249</v>
       </c>
@@ -27147,7 +27575,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>249</v>
       </c>
@@ -27247,7 +27675,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>249</v>
       </c>
@@ -27347,7 +27775,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>254</v>
       </c>
@@ -27447,7 +27875,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>254</v>
       </c>
@@ -27547,7 +27975,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>254</v>
       </c>
@@ -27647,7 +28075,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" ht="238" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>258</v>
       </c>
@@ -27732,7 +28160,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="59" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:58" ht="238" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>258</v>
       </c>
@@ -27817,7 +28245,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:58" ht="238" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>258</v>
       </c>
@@ -27902,7 +28330,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="1:58" s="39" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:58" s="39" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>262</v>
       </c>
@@ -27987,7 +28415,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="62" spans="1:58" s="39" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:58" s="39" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>262</v>
       </c>
@@ -28072,7 +28500,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="63" spans="1:58" s="39" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" s="39" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>262</v>
       </c>
@@ -28157,7 +28585,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="64" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>266</v>
       </c>
@@ -28249,7 +28677,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="65" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>266</v>
       </c>
@@ -28341,7 +28769,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>266</v>
       </c>
@@ -28433,7 +28861,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="67" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>271</v>
       </c>
@@ -28533,7 +28961,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>271</v>
       </c>
@@ -28633,7 +29061,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="69" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>274</v>
       </c>
@@ -28729,7 +29157,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>274</v>
       </c>
@@ -28825,7 +29253,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>277</v>
       </c>
@@ -28919,7 +29347,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>277</v>
       </c>
@@ -29013,7 +29441,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:58" s="38" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:58" s="38" customFormat="1" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="37" t="s">
         <v>281</v>
       </c>
@@ -29093,7 +29521,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>282</v>
       </c>
@@ -29178,7 +29606,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>282</v>
       </c>
@@ -29263,7 +29691,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>288</v>
       </c>
@@ -29361,7 +29789,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="77" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>288</v>
       </c>
@@ -29459,7 +29887,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="78" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>288</v>
       </c>
@@ -29491,7 +29919,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="79" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>288</v>
       </c>
@@ -29523,7 +29951,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="80" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>291</v>
       </c>
@@ -29620,7 +30048,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="81" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>291</v>
       </c>
@@ -29717,7 +30145,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>291</v>
       </c>
@@ -29755,7 +30183,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="83" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>291</v>
       </c>
@@ -29793,7 +30221,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="84" spans="1:58" s="38" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:58" s="38" customFormat="1" ht="196" x14ac:dyDescent="0.3">
       <c r="A84" s="37" t="s">
         <v>294</v>
       </c>
@@ -29881,7 +30309,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:58" s="38" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:58" s="38" customFormat="1" ht="196" x14ac:dyDescent="0.3">
       <c r="A85" s="37" t="s">
         <v>294</v>
       </c>
@@ -29919,7 +30347,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="86" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>296</v>
       </c>
@@ -30047,7 +30475,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="87" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>296</v>
       </c>
@@ -30160,7 +30588,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="88" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>296</v>
       </c>
@@ -30234,7 +30662,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="89" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>296</v>
       </c>
@@ -30341,7 +30769,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="90" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>296</v>
       </c>
@@ -30448,7 +30876,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>296</v>
       </c>
@@ -30522,7 +30950,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="92" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>296</v>
       </c>
@@ -30629,7 +31057,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="93" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>296</v>
       </c>
@@ -30736,7 +31164,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="94" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>296</v>
       </c>
@@ -30810,7 +31238,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="95" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>302</v>
       </c>
@@ -30887,7 +31315,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="96" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:58" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>305</v>
       </c>
@@ -30962,7 +31390,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>305</v>
       </c>
@@ -31036,7 +31464,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>305</v>
       </c>
@@ -31109,7 +31537,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>309</v>
       </c>
@@ -31182,7 +31610,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>309</v>
       </c>
@@ -31255,7 +31683,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>309</v>
       </c>
@@ -31325,7 +31753,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>312</v>
       </c>
@@ -31395,7 +31823,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>312</v>
       </c>
@@ -31465,7 +31893,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>312</v>
       </c>
@@ -31533,7 +31961,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="105" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>312</v>
       </c>
@@ -31603,7 +32031,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="106" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>312</v>
       </c>
@@ -31673,7 +32101,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>312</v>
       </c>
@@ -31741,7 +32169,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="108" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>312</v>
       </c>
@@ -31811,7 +32239,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="109" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>312</v>
       </c>
@@ -31881,7 +32309,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="110" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>312</v>
       </c>
@@ -31949,7 +32377,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="111" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>318</v>
       </c>
@@ -31995,7 +32423,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="112" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>318</v>
       </c>
@@ -32038,7 +32466,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="113" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>318</v>
       </c>
@@ -32085,7 +32513,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="114" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>318</v>
       </c>
@@ -32128,7 +32556,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="115" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>318</v>
       </c>
@@ -32165,7 +32593,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>328</v>
       </c>
@@ -32249,7 +32677,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="117" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>328</v>
       </c>
@@ -32320,7 +32748,7 @@
       </c>
       <c r="AL117" s="39"/>
     </row>
-    <row r="118" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>328</v>
       </c>
@@ -32391,7 +32819,7 @@
       </c>
       <c r="AL118" s="39"/>
     </row>
-    <row r="119" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>328</v>
       </c>
@@ -32475,7 +32903,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="120" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>328</v>
       </c>
@@ -32546,7 +32974,7 @@
       </c>
       <c r="AL120" s="39"/>
     </row>
-    <row r="121" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>328</v>
       </c>
@@ -32617,7 +33045,7 @@
       </c>
       <c r="AL121" s="39"/>
     </row>
-    <row r="122" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>332</v>
       </c>
@@ -32687,7 +33115,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="123" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>332</v>
       </c>
@@ -32758,7 +33186,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="124" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>332</v>
       </c>
@@ -32829,7 +33257,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="125" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>332</v>
       </c>
@@ -32899,7 +33327,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="126" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>332</v>
       </c>
@@ -32970,7 +33398,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="127" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>332</v>
       </c>
@@ -33041,7 +33469,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="128" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>342</v>
       </c>
@@ -33112,7 +33540,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>342</v>
       </c>
@@ -33183,7 +33611,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>348</v>
       </c>
@@ -33244,7 +33672,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>348</v>
       </c>
@@ -33306,7 +33734,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>348</v>
       </c>
@@ -33368,7 +33796,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>348</v>
       </c>
@@ -33436,7 +33864,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>348</v>
       </c>
@@ -33498,7 +33926,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>356</v>
       </c>
@@ -33559,7 +33987,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>356</v>
       </c>
@@ -33621,7 +34049,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>356</v>
       </c>
@@ -33689,7 +34117,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>356</v>
       </c>
@@ -33752,6 +34180,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BI138" xr:uid="{00000000-0001-0000-0500-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Nuclear"/>
+        <filter val="Nuclear CHP"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -36448,18 +36884,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36481,14 +36917,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B86DC8-3E2D-43CE-AD36-E688A1669DE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33403C9F-F7D8-4D9C-ABE9-5CDDE161B5F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -36502,4 +36930,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B86DC8-3E2D-43CE-AD36-E688A1669DE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added future power plants
</commit_message>
<xml_diff>
--- a/data/TradeRES_D2_1_Scenario_data_Corrected (1).xlsx
+++ b/data/TradeRES_D2_1_Scenario_data_Corrected (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5156885B-D11C-471F-AE37-C26A8A80AD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF914E7A-EBFC-4928-8BD1-F98B5E01F12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="903" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -1983,7 +1983,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2098,8 +2098,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2175,6 +2182,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -2308,13 +2320,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2439,11 +2452,19 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -22086,7 +22107,7 @@
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -22176,7 +22197,7 @@
         <v>84</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="0">ROUND(E3*3.6,2)</f>
+        <f t="shared" ref="I3:I10" si="0">ROUND(E3*3.6,2)</f>
         <v>3.96</v>
       </c>
       <c r="K3" t="s">
@@ -22569,7 +22590,7 @@
       </c>
       <c r="H18" s="36"/>
       <c r="I18" s="36">
-        <f t="shared" ref="I18:I29" si="1">ROUND(E18*3.6,2)</f>
+        <f t="shared" ref="I18:I25" si="1">ROUND(E18*3.6,2)</f>
         <v>3.96</v>
       </c>
       <c r="J18" s="36"/>
@@ -22939,28 +22960,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BI138"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K85" sqref="K85"/>
+      <selection pane="bottomRight" activeCell="Q145" sqref="Q145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.58203125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="13.58203125" customWidth="1"/>
-    <col min="7" max="7" width="6.58203125" customWidth="1"/>
-    <col min="8" max="8" width="4.75" customWidth="1"/>
-    <col min="9" max="9" width="6.58203125" customWidth="1"/>
-    <col min="10" max="10" width="4.75" customWidth="1"/>
-    <col min="11" max="11" width="6.58203125" customWidth="1"/>
-    <col min="12" max="12" width="4.75" customWidth="1"/>
-    <col min="13" max="13" width="6.58203125" customWidth="1"/>
-    <col min="14" max="14" width="4.75" customWidth="1"/>
-    <col min="15" max="15" width="6.58203125" customWidth="1"/>
-    <col min="16" max="16" width="4.75" customWidth="1"/>
-    <col min="17" max="20" width="6.58203125" customWidth="1"/>
+    <col min="3" max="5" width="13.58203125" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="18" width="6.6640625" customWidth="1"/>
+    <col min="19" max="20" width="6.58203125" customWidth="1"/>
     <col min="21" max="23" width="4.75" customWidth="1"/>
     <col min="24" max="37" width="6.58203125" customWidth="1"/>
     <col min="38" max="38" width="4.75" customWidth="1"/>
@@ -23282,7 +23295,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>164</v>
       </c>
@@ -23425,7 +23438,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>164</v>
       </c>
@@ -23568,7 +23581,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>164</v>
       </c>
@@ -23711,7 +23724,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>176</v>
       </c>
@@ -23854,7 +23867,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>176</v>
       </c>
@@ -23997,7 +24010,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>176</v>
       </c>
@@ -24140,7 +24153,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>180</v>
       </c>
@@ -24278,7 +24291,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>180</v>
       </c>
@@ -24416,7 +24429,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>186</v>
       </c>
@@ -24554,7 +24567,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>186</v>
       </c>
@@ -24692,7 +24705,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>191</v>
       </c>
@@ -24832,7 +24845,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>191</v>
       </c>
@@ -24972,7 +24985,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>191</v>
       </c>
@@ -25112,7 +25125,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>198</v>
       </c>
@@ -25180,7 +25193,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>198</v>
       </c>
@@ -25248,7 +25261,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>198</v>
       </c>
@@ -25316,7 +25329,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>206</v>
       </c>
@@ -25384,7 +25397,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>206</v>
       </c>
@@ -25452,7 +25465,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>206</v>
       </c>
@@ -25520,7 +25533,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>210</v>
       </c>
@@ -25589,7 +25602,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>214</v>
       </c>
@@ -25658,7 +25671,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>216</v>
       </c>
@@ -25727,7 +25740,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>218</v>
       </c>
@@ -25795,7 +25808,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>210</v>
       </c>
@@ -25864,7 +25877,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>214</v>
       </c>
@@ -25933,7 +25946,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>216</v>
       </c>
@@ -26002,7 +26015,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>218</v>
       </c>
@@ -26070,7 +26083,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>210</v>
       </c>
@@ -26139,7 +26152,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>214</v>
       </c>
@@ -26208,7 +26221,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>216</v>
       </c>
@@ -26277,7 +26290,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>218</v>
       </c>
@@ -26348,7 +26361,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>221</v>
       </c>
@@ -26421,7 +26434,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>221</v>
       </c>
@@ -26493,7 +26506,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="36" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>224</v>
       </c>
@@ -26595,7 +26608,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>224</v>
       </c>
@@ -26697,7 +26710,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:61" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>227</v>
       </c>
@@ -26795,7 +26808,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="1:61" s="69" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:61" s="69" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="68" t="s">
         <v>227</v>
       </c>
@@ -26893,7 +26906,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="40" spans="1:61" s="38" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:61" s="38" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="37" t="s">
         <v>82</v>
       </c>
@@ -26982,7 +26995,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:61" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:61" s="36" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="34" t="s">
         <v>232</v>
       </c>
@@ -27004,7 +27017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:61" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:61" s="36" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="34" t="s">
         <v>232</v>
       </c>
@@ -27026,7 +27039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:61" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:61" s="36" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="34" t="s">
         <v>232</v>
       </c>
@@ -27045,7 +27058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>236</v>
       </c>
@@ -27098,7 +27111,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>236</v>
       </c>
@@ -27151,7 +27164,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="46" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>241</v>
       </c>
@@ -27204,7 +27217,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="47" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>241</v>
       </c>
@@ -27257,7 +27270,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="48" spans="1:61" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>244</v>
       </c>
@@ -27322,7 +27335,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="49" spans="1:58" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>244</v>
       </c>
@@ -27387,7 +27400,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="50" spans="1:58" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>247</v>
       </c>
@@ -27431,7 +27444,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:58" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>247</v>
       </c>
@@ -27475,7 +27488,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>249</v>
       </c>
@@ -27575,7 +27588,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>249</v>
       </c>
@@ -27675,7 +27688,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>249</v>
       </c>
@@ -27775,7 +27788,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:58" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>254</v>
       </c>
@@ -27875,7 +27888,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>254</v>
       </c>
@@ -27975,7 +27988,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:58" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>254</v>
       </c>
@@ -28075,7 +28088,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="1:58" ht="238" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>258</v>
       </c>
@@ -28160,7 +28173,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="59" spans="1:58" ht="238" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:58" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>258</v>
       </c>
@@ -28245,7 +28258,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:58" ht="238" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:58" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>258</v>
       </c>
@@ -28330,7 +28343,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="1:58" s="39" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:58" s="39" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>262</v>
       </c>
@@ -28415,7 +28428,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="62" spans="1:58" s="39" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:58" s="39" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>262</v>
       </c>
@@ -28500,7 +28513,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="63" spans="1:58" s="39" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" s="39" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>262</v>
       </c>
@@ -28585,7 +28598,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="64" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>266</v>
       </c>
@@ -28677,7 +28690,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="65" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>266</v>
       </c>
@@ -28769,7 +28782,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>266</v>
       </c>
@@ -28861,7 +28874,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="67" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>271</v>
       </c>
@@ -28961,7 +28974,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>271</v>
       </c>
@@ -29061,7 +29074,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="69" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>274</v>
       </c>
@@ -29157,7 +29170,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>274</v>
       </c>
@@ -29253,7 +29266,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>277</v>
       </c>
@@ -29347,7 +29360,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>277</v>
       </c>
@@ -29441,7 +29454,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:58" s="38" customFormat="1" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:58" s="38" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="37" t="s">
         <v>281</v>
       </c>
@@ -29521,7 +29534,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>282</v>
       </c>
@@ -29606,7 +29619,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>282</v>
       </c>
@@ -29691,7 +29704,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>288</v>
       </c>
@@ -29789,7 +29802,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="77" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>288</v>
       </c>
@@ -29887,7 +29900,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="78" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>288</v>
       </c>
@@ -29919,7 +29932,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="79" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>288</v>
       </c>
@@ -29951,7 +29964,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="80" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>291</v>
       </c>
@@ -30048,7 +30061,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="81" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>291</v>
       </c>
@@ -30145,7 +30158,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>291</v>
       </c>
@@ -30183,7 +30196,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="83" spans="1:58" ht="196" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>291</v>
       </c>
@@ -30221,7 +30234,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="84" spans="1:58" s="38" customFormat="1" ht="196" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:58" s="38" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="37" t="s">
         <v>294</v>
       </c>
@@ -30309,7 +30322,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:58" s="38" customFormat="1" ht="196" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:58" s="38" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="37" t="s">
         <v>294</v>
       </c>
@@ -30347,135 +30360,135 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="86" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
+    <row r="86" spans="1:58" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+      <c r="A86" s="74" t="s">
         <v>296</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="74" t="s">
         <v>297</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="75">
         <v>2030</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="75">
         <v>21</v>
       </c>
-      <c r="H86" s="39" t="s">
+      <c r="H86" s="76" t="s">
         <v>298</v>
       </c>
-      <c r="I86">
+      <c r="I86" s="75">
         <v>160</v>
       </c>
-      <c r="J86" t="s">
+      <c r="J86" s="75" t="s">
         <v>299</v>
       </c>
-      <c r="K86">
+      <c r="K86" s="75">
         <v>540</v>
       </c>
-      <c r="L86" t="s">
+      <c r="L86" s="75" t="s">
         <v>299</v>
       </c>
-      <c r="M86">
+      <c r="M86" s="75">
         <v>1.8</v>
       </c>
-      <c r="N86" t="s">
+      <c r="N86" s="75" t="s">
         <v>299</v>
       </c>
-      <c r="O86">
+      <c r="O86" s="75">
         <v>25</v>
       </c>
-      <c r="P86" s="39" t="s">
+      <c r="P86" s="76" t="s">
         <v>298</v>
       </c>
-      <c r="Q86">
+      <c r="Q86" s="75">
         <v>20</v>
       </c>
-      <c r="R86">
+      <c r="R86" s="75">
         <v>7</v>
       </c>
-      <c r="S86" s="31">
+      <c r="S86" s="77">
         <f>IFERROR(ROUND(-PMT(R86/100,Q86,1),6),0)</f>
         <v>9.4393000000000005E-2</v>
       </c>
-      <c r="T86" s="31">
+      <c r="T86" s="77">
         <f t="shared" si="15"/>
         <v>15102.880000000001</v>
       </c>
-      <c r="U86" t="s">
+      <c r="U86" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="V86" s="41">
+      <c r="V86" s="78">
         <f>0.1*7</f>
         <v>0.70000000000000007</v>
       </c>
-      <c r="W86" s="39" t="s">
+      <c r="W86" s="76" t="s">
         <v>298</v>
       </c>
-      <c r="X86" s="41"/>
-      <c r="Y86" s="41"/>
-      <c r="Z86" s="41"/>
-      <c r="AA86" s="41"/>
-      <c r="AB86" s="41"/>
-      <c r="AC86" s="41"/>
-      <c r="AD86" s="41"/>
-      <c r="AE86" s="41"/>
-      <c r="AF86" s="41"/>
-      <c r="AG86" s="41"/>
-      <c r="AH86" s="41"/>
-      <c r="AI86" s="41"/>
-      <c r="AJ86" s="41"/>
-      <c r="AK86" s="41"/>
-      <c r="AL86" s="41"/>
-      <c r="AM86">
+      <c r="X86" s="78"/>
+      <c r="Y86" s="78"/>
+      <c r="Z86" s="78"/>
+      <c r="AA86" s="78"/>
+      <c r="AB86" s="78"/>
+      <c r="AC86" s="78"/>
+      <c r="AD86" s="78"/>
+      <c r="AE86" s="78"/>
+      <c r="AF86" s="78"/>
+      <c r="AG86" s="78"/>
+      <c r="AH86" s="78"/>
+      <c r="AI86" s="78"/>
+      <c r="AJ86" s="78"/>
+      <c r="AK86" s="78"/>
+      <c r="AL86" s="78"/>
+      <c r="AM86" s="75">
         <v>97.5</v>
       </c>
-      <c r="AN86">
+      <c r="AN86" s="75">
         <v>95.5</v>
       </c>
-      <c r="AP86" s="39" t="s">
+      <c r="AP86" s="76" t="s">
         <v>300</v>
       </c>
-      <c r="AU86">
-        <v>0</v>
-      </c>
-      <c r="AV86">
-        <v>0</v>
-      </c>
-      <c r="AX86">
+      <c r="AU86" s="75">
+        <v>0</v>
+      </c>
+      <c r="AV86" s="75">
+        <v>0</v>
+      </c>
+      <c r="AX86" s="75">
         <v>100</v>
       </c>
-      <c r="AY86">
+      <c r="AY86" s="75">
         <v>100</v>
       </c>
-      <c r="AZ86">
+      <c r="AZ86" s="75">
         <v>100</v>
       </c>
-      <c r="BA86">
+      <c r="BA86" s="75">
         <v>100</v>
       </c>
-      <c r="BB86">
+      <c r="BB86" s="75">
         <v>100</v>
       </c>
-      <c r="BC86">
+      <c r="BC86" s="75">
         <v>100</v>
       </c>
-      <c r="BD86">
+      <c r="BD86" s="75">
         <v>100</v>
       </c>
-      <c r="BE86">
+      <c r="BE86" s="75">
         <v>100</v>
       </c>
-      <c r="BF86" t="s">
+      <c r="BF86" s="75" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="87" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:58" ht="28" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>296</v>
       </c>
@@ -30588,7 +30601,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="88" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:58" ht="28" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>296</v>
       </c>
@@ -30662,7 +30675,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="89" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:58" ht="28" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>296</v>
       </c>
@@ -30769,7 +30782,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="90" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:58" ht="28" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>296</v>
       </c>
@@ -30876,7 +30889,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:58" ht="28" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>296</v>
       </c>
@@ -30950,7 +30963,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="92" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:58" ht="28" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>296</v>
       </c>
@@ -31057,7 +31070,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="93" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:58" ht="28" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>296</v>
       </c>
@@ -31164,7 +31177,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="94" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:58" ht="28" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>296</v>
       </c>
@@ -31238,7 +31251,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="95" spans="1:58" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:58" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>302</v>
       </c>
@@ -31315,7 +31328,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="96" spans="1:58" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:58" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>305</v>
       </c>
@@ -31390,7 +31403,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="97" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>305</v>
       </c>
@@ -31464,7 +31477,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="98" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>305</v>
       </c>
@@ -31537,7 +31550,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="99" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>309</v>
       </c>
@@ -31610,7 +31623,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="100" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>309</v>
       </c>
@@ -31683,7 +31696,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="101" spans="1:42" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>309</v>
       </c>
@@ -31753,7 +31766,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="102" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>312</v>
       </c>
@@ -31823,7 +31836,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="103" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>312</v>
       </c>
@@ -31893,7 +31906,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="104" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>312</v>
       </c>
@@ -31961,7 +31974,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="105" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>312</v>
       </c>
@@ -32031,7 +32044,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="106" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>312</v>
       </c>
@@ -32101,7 +32114,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="107" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>312</v>
       </c>
@@ -32169,7 +32182,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="108" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>312</v>
       </c>
@@ -32239,7 +32252,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="109" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>312</v>
       </c>
@@ -32309,7 +32322,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="110" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>312</v>
       </c>
@@ -32377,7 +32390,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="111" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>318</v>
       </c>
@@ -32423,7 +32436,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="112" spans="1:42" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>318</v>
       </c>
@@ -32466,7 +32479,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="113" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>318</v>
       </c>
@@ -32513,7 +32526,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="114" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>318</v>
       </c>
@@ -32556,7 +32569,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="115" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>318</v>
       </c>
@@ -32593,7 +32606,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>328</v>
       </c>
@@ -32677,7 +32690,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="117" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>328</v>
       </c>
@@ -32748,7 +32761,7 @@
       </c>
       <c r="AL117" s="39"/>
     </row>
-    <row r="118" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>328</v>
       </c>
@@ -32819,7 +32832,7 @@
       </c>
       <c r="AL118" s="39"/>
     </row>
-    <row r="119" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>328</v>
       </c>
@@ -32903,7 +32916,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="120" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>328</v>
       </c>
@@ -32974,7 +32987,7 @@
       </c>
       <c r="AL120" s="39"/>
     </row>
-    <row r="121" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>328</v>
       </c>
@@ -33045,7 +33058,7 @@
       </c>
       <c r="AL121" s="39"/>
     </row>
-    <row r="122" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>332</v>
       </c>
@@ -33115,7 +33128,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="123" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>332</v>
       </c>
@@ -33186,7 +33199,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="124" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>332</v>
       </c>
@@ -33257,7 +33270,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="125" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>332</v>
       </c>
@@ -33327,7 +33340,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="126" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>332</v>
       </c>
@@ -33398,7 +33411,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="127" spans="1:44" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>332</v>
       </c>
@@ -33469,7 +33482,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="128" spans="1:44" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>342</v>
       </c>
@@ -33540,7 +33553,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>342</v>
       </c>
@@ -33611,7 +33624,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>348</v>
       </c>
@@ -33672,7 +33685,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>348</v>
       </c>
@@ -33734,7 +33747,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>348</v>
       </c>
@@ -33796,7 +33809,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>348</v>
       </c>
@@ -33864,7 +33877,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>348</v>
       </c>
@@ -33926,7 +33939,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>356</v>
       </c>
@@ -33987,7 +34000,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>356</v>
       </c>
@@ -34049,7 +34062,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>356</v>
       </c>
@@ -34117,7 +34130,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>356</v>
       </c>
@@ -34183,8 +34196,7 @@
   <autoFilter ref="A1:BI138" xr:uid="{00000000-0001-0000-0500-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Nuclear"/>
-        <filter val="Nuclear CHP"/>
+        <filter val="Lithium-ion battery"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -36884,18 +36896,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36917,6 +36929,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B86DC8-3E2D-43CE-AD36-E688A1669DE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33403C9F-F7D8-4D9C-ABE9-5CDDE161B5F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -36930,12 +36950,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B86DC8-3E2D-43CE-AD36-E688A1669DE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>